<commit_message>
Mostly html and css changes.
</commit_message>
<xml_diff>
--- a/Carter/Excel Wine Dashboard Prototype.xlsx
+++ b/Carter/Excel Wine Dashboard Prototype.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carter\Desktop\Project 2\Group-Project2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carter\Desktop\Project 2\Group-Project2\Carter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF14189-F985-4F53-9E75-074D6CD20180}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE0F947-EDAF-4BCA-9A16-5B4A9B2BDFEC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="57">
   <si>
     <t>Variety</t>
   </si>
@@ -200,6 +200,33 @@
   </si>
   <si>
     <t>Wine Variety Dashboard (Prototype)</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Updated NAV Bar</t>
+  </si>
+  <si>
+    <t>Updated Links</t>
+  </si>
+  <si>
+    <t>About</t>
+  </si>
+  <si>
+    <t>Created</t>
+  </si>
+  <si>
+    <t>Total Reviews by Country (map)</t>
+  </si>
+  <si>
+    <t>Country Level Summary</t>
+  </si>
+  <si>
+    <t>Wine Dashboard by Variety</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -472,7 +499,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Syrah</c:v>
+                  <c:v>Pinot Noir</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -526,7 +553,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -538,7 +565,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -686,7 +713,7 @@
                 <c:formatCode>"$"#,##0_);\("$"#,##0\);"$"#,##0_);@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>31</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -758,7 +785,7 @@
                 <c:formatCode>"$"#,##0_);\("$"#,##0\);"$"#,##0_);@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -830,7 +857,7 @@
                 <c:formatCode>"$"#,##0_);\("$"#,##0\);"$"#,##0_);@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1118,7 +1145,7 @@
                 <c:formatCode>"$"#,##0_);\("$"#,##0\);"$"#,##0_);@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1190,7 +1217,7 @@
                 <c:formatCode>"$"#,##0_);\("$"#,##0\);"$"#,##0_);@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1262,7 +1289,7 @@
                 <c:formatCode>"$"#,##0_);\("$"#,##0\);"$"#,##0_);@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1334,7 +1361,7 @@
                 <c:formatCode>"$"#,##0_);\("$"#,##0\);"$"#,##0_);@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="2">
-                  <c:v>36</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1482,7 +1509,7 @@
                 <c:formatCode>"$"#,##0_);\("$"#,##0\);"$"#,##0_);@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="3">
-                  <c:v>36</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1554,7 +1581,7 @@
                 <c:formatCode>"$"#,##0_);\("$"#,##0\);"$"#,##0_);@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="3">
-                  <c:v>26</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1698,7 +1725,7 @@
                 <c:formatCode>"$"#,##0_);\("$"#,##0\);"$"#,##0_);@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="4">
-                  <c:v>55</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1770,7 +1797,7 @@
                 <c:formatCode>"$"#,##0_);\("$"#,##0\);"$"#,##0_);@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="4">
-                  <c:v>43</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1842,7 +1869,7 @@
                 <c:formatCode>"$"#,##0_);\("$"#,##0\);"$"#,##0_);@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="4">
-                  <c:v>43</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1924,7 +1951,7 @@
                 <c:formatCode>"$"#,##0_);\("$"#,##0\);"$"#,##0_);@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="4">
-                  <c:v>43</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1996,7 +2023,7 @@
                 <c:formatCode>"$"#,##0_);\("$"#,##0\);"$"#,##0_);@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2506,8 +2533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BJ66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2559,7 +2586,7 @@
       </c>
       <c r="AB1" t="str">
         <f>B6</f>
-        <v>Syrah</v>
+        <v>Pinot Noir</v>
       </c>
       <c r="AE1" t="s">
         <v>0</v>
@@ -2584,79 +2611,79 @@
       </c>
       <c r="AR1" t="str">
         <f>AR9&amp;$B$6</f>
-        <v>1USASyrah</v>
+        <v>1USAPinot Noir</v>
       </c>
       <c r="AS1" t="str">
         <f t="shared" ref="AS1:BJ1" si="0">AS9&amp;$B$6</f>
-        <v>2USASyrah</v>
+        <v>2USAPinot Noir</v>
       </c>
       <c r="AT1" t="str">
         <f t="shared" si="0"/>
-        <v>1FranceSyrah</v>
+        <v>1FrancePinot Noir</v>
       </c>
       <c r="AU1" t="str">
         <f t="shared" si="0"/>
-        <v>2FranceSyrah</v>
+        <v>2FrancePinot Noir</v>
       </c>
       <c r="AV1" t="str">
         <f t="shared" si="0"/>
-        <v>3FranceSyrah</v>
+        <v>3FrancePinot Noir</v>
       </c>
       <c r="AW1" t="str">
         <f t="shared" si="0"/>
-        <v>4FranceSyrah</v>
+        <v>4FrancePinot Noir</v>
       </c>
       <c r="AX1" t="str">
         <f t="shared" si="0"/>
-        <v>1ItalySyrah</v>
+        <v>1ItalyPinot Noir</v>
       </c>
       <c r="AY1" t="str">
         <f t="shared" si="0"/>
-        <v>2ItalySyrah</v>
+        <v>2ItalyPinot Noir</v>
       </c>
       <c r="AZ1" t="str">
         <f t="shared" si="0"/>
-        <v>3ItalySyrah</v>
+        <v>3ItalyPinot Noir</v>
       </c>
       <c r="BA1" t="str">
         <f t="shared" si="0"/>
-        <v>4ItalySyrah</v>
+        <v>4ItalyPinot Noir</v>
       </c>
       <c r="BB1" t="str">
         <f t="shared" si="0"/>
-        <v>1ArgentinaSyrah</v>
+        <v>1ArgentinaPinot Noir</v>
       </c>
       <c r="BC1" t="str">
         <f t="shared" si="0"/>
-        <v>2ArgentinaSyrah</v>
+        <v>2ArgentinaPinot Noir</v>
       </c>
       <c r="BD1" t="str">
         <f t="shared" si="0"/>
-        <v>3ArgentinaSyrah</v>
+        <v>3ArgentinaPinot Noir</v>
       </c>
       <c r="BE1" t="str">
         <f t="shared" si="0"/>
-        <v>4ArgentinaSyrah</v>
+        <v>4ArgentinaPinot Noir</v>
       </c>
       <c r="BF1" t="str">
         <f t="shared" si="0"/>
-        <v>1AustraliaSyrah</v>
+        <v>1AustraliaPinot Noir</v>
       </c>
       <c r="BG1" t="str">
         <f t="shared" si="0"/>
-        <v>2AustraliaSyrah</v>
+        <v>2AustraliaPinot Noir</v>
       </c>
       <c r="BH1" t="str">
         <f t="shared" si="0"/>
-        <v>3AustraliaSyrah</v>
+        <v>3AustraliaPinot Noir</v>
       </c>
       <c r="BI1" t="str">
         <f t="shared" si="0"/>
-        <v>4AustraliaSyrah</v>
+        <v>4AustraliaPinot Noir</v>
       </c>
       <c r="BJ1" t="str">
         <f t="shared" si="0"/>
-        <v>5AustraliaSyrah</v>
+        <v>5AustraliaPinot Noir</v>
       </c>
     </row>
     <row r="2" spans="2:62" x14ac:dyDescent="0.35">
@@ -2677,7 +2704,7 @@
       </c>
       <c r="AB2">
         <f>COUNTIFS(U:U,AA2,V:V,$AB$1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE2" t="s">
         <v>9</v>
@@ -2706,11 +2733,11 @@
       </c>
       <c r="AR2" s="16">
         <f>IFERROR(VLOOKUP(AR$1,$AJ:$AK,2,FALSE),"")</f>
-        <v>31</v>
-      </c>
-      <c r="AS2" s="16">
+        <v>12</v>
+      </c>
+      <c r="AS2" s="16" t="str">
         <f>IFERROR(VLOOKUP(AS$1,$AJ:$AK,2,FALSE),"")</f>
-        <v>20</v>
+        <v/>
       </c>
       <c r="AT2" s="16"/>
       <c r="AU2" s="16"/>
@@ -2779,7 +2806,7 @@
       <c r="AS3" s="16"/>
       <c r="AT3" s="16">
         <f>IFERROR(VLOOKUP(AT$1,$AJ:$AK,2,FALSE),"")</f>
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="AU3" s="16" t="str">
         <f>IFERROR(VLOOKUP(AU$1,$AJ:$AK,2,FALSE),"")</f>
@@ -2867,19 +2894,19 @@
       <c r="AW4" s="16"/>
       <c r="AX4" s="16">
         <f>IFERROR(VLOOKUP(AX$1,$AJ:$AK,2,FALSE),"")</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AY4" s="16">
         <f>IFERROR(VLOOKUP(AY$1,$AJ:$AK,2,FALSE),"")</f>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="AZ4" s="16">
         <f>IFERROR(VLOOKUP(AZ$1,$AJ:$AK,2,FALSE),"")</f>
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="BA4" s="16">
         <f>IFERROR(VLOOKUP(BA$1,$AJ:$AK,2,FALSE),"")</f>
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="BB4" s="16"/>
       <c r="BC4" s="16"/>
@@ -2963,11 +2990,11 @@
       </c>
       <c r="BC5" s="16">
         <f>IFERROR(VLOOKUP(BC$1,$AJ:$AK,2,FALSE),"")</f>
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="BD5" s="16">
         <f>IFERROR(VLOOKUP(BD$1,$AJ:$AK,2,FALSE),"")</f>
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="BE5" s="16" t="str">
         <f>IFERROR(VLOOKUP(BE$1,$AJ:$AK,2,FALSE),"")</f>
@@ -2981,7 +3008,7 @@
     </row>
     <row r="6" spans="2:62" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -2990,7 +3017,7 @@
       </c>
       <c r="K6" s="7">
         <f>AVERAGEIF(V:V,$B$6,W:W)</f>
-        <v>33.714285714285715</v>
+        <v>26.642857142857142</v>
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -3011,7 +3038,7 @@
       </c>
       <c r="AB6">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AE6" t="s">
         <v>13</v>
@@ -3054,23 +3081,23 @@
       <c r="BE6" s="16"/>
       <c r="BF6" s="16">
         <f>IFERROR(VLOOKUP(BF$1,$AJ:$AK,2,FALSE),"")</f>
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="BG6" s="16">
         <f>IFERROR(VLOOKUP(BG$1,$AJ:$AK,2,FALSE),"")</f>
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="BH6" s="16">
         <f>IFERROR(VLOOKUP(BH$1,$AJ:$AK,2,FALSE),"")</f>
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="BI6" s="16">
         <f>IFERROR(VLOOKUP(BI$1,$AJ:$AK,2,FALSE),"")</f>
-        <v>43</v>
-      </c>
-      <c r="BJ6" s="16" t="str">
+        <v>14</v>
+      </c>
+      <c r="BJ6" s="16">
         <f>IFERROR(VLOOKUP(BJ$1,$AJ:$AK,2,FALSE),"")</f>
-        <v/>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:62" x14ac:dyDescent="0.35">
@@ -3081,7 +3108,7 @@
       </c>
       <c r="K7" s="7">
         <f t="array" ref="K7">MAX(IF(V:V=B6,W:W))</f>
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
@@ -3147,7 +3174,7 @@
       </c>
       <c r="K8" s="8">
         <f t="array" ref="K8">MIN(IF(V:V=B6,W:W))</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -5316,12 +5343,75 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>